<commit_message>
Dash DI - V1
</commit_message>
<xml_diff>
--- a/Dados/Ativos_Sem_Codigo.xlsx
+++ b/Dados/Ativos_Sem_Codigo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Sub Classe</t>
   </si>
@@ -34,52 +34,37 @@
     <t>COD_XP</t>
   </si>
   <si>
-    <t>Títulos Privados</t>
-  </si>
-  <si>
-    <t>Letra Financeira</t>
+    <t>LFSN</t>
   </si>
   <si>
     <t>CDB</t>
   </si>
   <si>
-    <t>LF00240072E</t>
-  </si>
-  <si>
-    <t>CDB3251WXH0</t>
-  </si>
-  <si>
-    <t>LF0024008OB</t>
-  </si>
-  <si>
-    <t>LF0024007Y4</t>
-  </si>
-  <si>
-    <t>CDB925CDN0L</t>
+    <t>LFSN1800DIG</t>
+  </si>
+  <si>
+    <t>CDB725BEF4D</t>
+  </si>
+  <si>
+    <t>CDB725BEF4B</t>
+  </si>
+  <si>
+    <t>CDB725BEF4E</t>
+  </si>
+  <si>
+    <t>CDB725BEF4C</t>
+  </si>
+  <si>
+    <t>FIRF GERAES</t>
   </si>
   <si>
     <t>BMG SEG</t>
   </si>
   <si>
-    <t>JERA2026</t>
-  </si>
-  <si>
-    <t>REAL FIM</t>
-  </si>
-  <si>
-    <t>FIRF GERAES</t>
-  </si>
-  <si>
-    <t>BBRASIL FIM CP RESP</t>
-  </si>
-  <si>
-    <t>BH FIRF INFRA</t>
-  </si>
-  <si>
     <t>FIRF GERAES 30</t>
   </si>
   <si>
-    <t>TOPAZIO INFRA</t>
+    <t>HORIZONTE</t>
   </si>
 </sst>
 </file>
@@ -441,7 +426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -472,52 +457,52 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2">
-        <v>46083</v>
+        <v>46237</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2">
-        <v>46083</v>
+        <v>45941</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="2">
-        <v>46454</v>
+        <v>45941</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2">
-        <v>46454</v>
+        <v>45941</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -525,128 +510,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2">
-        <v>46454</v>
+        <v>45941</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2">
-        <v>46104</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2">
-        <v>46104</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="2">
-        <v>46097</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2">
-        <v>46013</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2">
-        <v>46454</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="2">
-        <v>46454</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="2">
-        <v>46454</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="2">
-        <v>46454</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>